<commit_message>
Complete check permission for "Product management" group.
</commit_message>
<xml_diff>
--- a/src/main/resources/uploadfile/import_product/import_product.xlsx
+++ b/src/main/resources/uploadfile/import_product/import_product.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation-Local\src\main\resources\uploadfile\import_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63173F22-4577-423D-ADA6-CC835B67322C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0392283-1D18-4F33-8B79-6A8067957415}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="7500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>Do not input</t>
   </si>
@@ -490,15 +490,11 @@
       <t>(Mandatory)</t>
     </r>
   </si>
-  <si>
-    <t>33218</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -958,39 +954,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.109375"/>
-    <col min="2" max="3" customWidth="true" width="16.33203125"/>
-    <col min="4" max="4" customWidth="true" width="35.88671875"/>
-    <col min="5" max="5" customWidth="true" width="14.44140625"/>
-    <col min="6" max="6" customWidth="true" width="31.33203125"/>
-    <col min="7" max="7" customWidth="true" width="15.33203125"/>
-    <col min="8" max="8" customWidth="true" width="17.33203125"/>
-    <col min="9" max="9" customWidth="true" width="16.109375"/>
-    <col min="10" max="10" customWidth="true" width="17.33203125"/>
-    <col min="11" max="11" customWidth="true" width="39.5546875"/>
-    <col min="12" max="13" customWidth="true" width="21.33203125"/>
-    <col min="14" max="14" customWidth="true" width="20.6640625"/>
-    <col min="15" max="15" customWidth="true" width="26.88671875"/>
-    <col min="16" max="17" customWidth="true" width="32.88671875"/>
-    <col min="18" max="18" customWidth="true" width="29.6640625"/>
-    <col min="19" max="19" customWidth="true" width="19.33203125"/>
-    <col min="20" max="20" customWidth="true" width="17.88671875"/>
-    <col min="21" max="21" customWidth="true" width="22.109375"/>
-    <col min="22" max="22" customWidth="true" width="22.44140625"/>
-    <col min="23" max="23" customWidth="true" width="23.109375"/>
-    <col min="24" max="24" customWidth="true" width="25.109375"/>
-    <col min="25" max="25" customWidth="true" width="21.44140625"/>
-    <col min="26" max="26" customWidth="true" width="24.6640625"/>
-    <col min="27" max="27" customWidth="true" width="17.6640625"/>
-    <col min="28" max="28" customWidth="true" width="19.109375"/>
-    <col min="29" max="29" customWidth="true" width="21.5546875"/>
-    <col min="30" max="30" customWidth="true" width="23.6640625"/>
-    <col min="31" max="31" customWidth="true" width="10.44140625"/>
-    <col min="32" max="32" customWidth="true" width="17.33203125"/>
-    <col min="33" max="33" customWidth="true" width="15.44140625"/>
-    <col min="34" max="34" customWidth="true" width="24.109375"/>
-    <col min="35" max="35" customWidth="true" width="14.6640625"/>
-    <col min="36" max="36" customWidth="true" width="20.33203125"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="39.5546875" customWidth="1"/>
+    <col min="12" max="13" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="26.88671875" customWidth="1"/>
+    <col min="16" max="17" width="32.88671875" customWidth="1"/>
+    <col min="18" max="18" width="29.6640625" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" customWidth="1"/>
+    <col min="20" max="20" width="17.88671875" customWidth="1"/>
+    <col min="21" max="21" width="22.109375" customWidth="1"/>
+    <col min="22" max="22" width="22.44140625" customWidth="1"/>
+    <col min="23" max="23" width="23.109375" customWidth="1"/>
+    <col min="24" max="24" width="25.109375" customWidth="1"/>
+    <col min="25" max="25" width="21.44140625" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" customWidth="1"/>
+    <col min="27" max="27" width="17.6640625" customWidth="1"/>
+    <col min="28" max="28" width="19.109375" customWidth="1"/>
+    <col min="29" max="29" width="21.5546875" customWidth="1"/>
+    <col min="30" max="30" width="23.6640625" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" customWidth="1"/>
+    <col min="32" max="32" width="17.33203125" customWidth="1"/>
+    <col min="33" max="33" width="15.44140625" customWidth="1"/>
+    <col min="34" max="34" width="24.109375" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="189" customHeight="1">
@@ -1241,9 +1237,6 @@
       </c>
       <c r="P3" s="5">
         <v>1000</v>
-      </c>
-      <c r="Q3" t="s" s="0">
-        <v>71</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>68</v>

</xml_diff>